<commit_message>
Lots of edits to get basic scene started, also added unit testing and other files - not all of them used yet
</commit_message>
<xml_diff>
--- a/documents/MasterStoryList.xlsx
+++ b/documents/MasterStoryList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>User Story</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Iteration</t>
+  </si>
+  <si>
+    <t>1. Can change the color of a light 2. Invalid color input has no effect on color of light</t>
+  </si>
+  <si>
+    <t>Need to be able to create light, set color, and see result</t>
   </si>
 </sst>
 </file>
@@ -583,13 +589,15 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
@@ -605,14 +613,14 @@
       <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -621,6 +629,12 @@
       </c>
       <c r="C2">
         <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>